<commit_message>
Added info in extent report
</commit_message>
<xml_diff>
--- a/src/resources/CurrencyConversionData.xlsx
+++ b/src/resources/CurrencyConversionData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Awani\Desktop\Rockall\rockall\src\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD959835-C349-4F38-BBBD-E6B4AB94B7EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E7ADE76-A14B-4157-A7B0-705570A118A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3705" yWindow="780" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t>TestCase Name</t>
   </si>
@@ -54,10 +54,31 @@
     <t>INR</t>
   </si>
   <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>.01</t>
+    <t>TC_03</t>
+  </si>
+  <si>
+    <t>TC_04</t>
+  </si>
+  <si>
+    <t>TC_05</t>
+  </si>
+  <si>
+    <t>90000</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>85000</t>
+  </si>
+  <si>
+    <t>100000</t>
+  </si>
+  <si>
+    <t>USD</t>
+  </si>
+  <si>
+    <t>8797</t>
   </si>
 </sst>
 </file>
@@ -392,10 +413,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -426,13 +447,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -440,13 +461,55 @@
         <v>7</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>6</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>